<commit_message>
fixing issue with now outputting all station numbers. leveraging provided station id instead of index for the title
</commit_message>
<xml_diff>
--- a/template_excel.xlsx
+++ b/template_excel.xlsx
@@ -1,19 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21810"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\repo\ei-automation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\code\ei-automation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8D7BCF41-0CA5-43BD-BF7A-76EC693A6223}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92A3629B-D182-4C01-AD7F-22A997BDB1B8}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12225" firstSheet="1" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="24496" windowHeight="15796" firstSheet="1" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="User Input" sheetId="1" r:id="rId1"/>
+    <sheet name="User Input" sheetId="1" state="hidden" r:id="rId1"/>
     <sheet name="UI" sheetId="37" r:id="rId2"/>
     <sheet name="Formula Sheet" sheetId="38" r:id="rId3"/>
   </sheets>
@@ -29,7 +29,9 @@
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
         <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
         <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
       </xcalcf:calcFeatures>
     </ext>
   </extLst>
@@ -3306,16 +3308,16 @@
       <selection activeCell="H4" sqref="H4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="2" max="2" width="9.5703125" customWidth="1"/>
-    <col min="3" max="3" width="9.42578125" customWidth="1"/>
-    <col min="7" max="7" width="14.42578125" customWidth="1"/>
-    <col min="8" max="8" width="13.28515625" customWidth="1"/>
-    <col min="9" max="9" width="14.28515625" customWidth="1"/>
+    <col min="2" max="2" width="9.59765625" customWidth="1"/>
+    <col min="3" max="3" width="9.3984375" customWidth="1"/>
+    <col min="7" max="7" width="14.3984375" customWidth="1"/>
+    <col min="8" max="8" width="13.265625" customWidth="1"/>
+    <col min="9" max="9" width="14.265625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="1" spans="2:26" x14ac:dyDescent="0.45">
       <c r="D1" t="s">
         <v>16</v>
       </c>
@@ -3330,7 +3332,7 @@
       </c>
       <c r="Z1" s="3"/>
     </row>
-    <row r="2" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:26" x14ac:dyDescent="0.45">
       <c r="B2" s="9" t="s">
         <v>9</v>
       </c>
@@ -3351,7 +3353,7 @@
       <c r="Y2" s="3"/>
       <c r="Z2" s="3"/>
     </row>
-    <row r="3" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F3" t="str">
         <f t="shared" si="0"/>
         <v>ST2</v>
@@ -3365,7 +3367,7 @@
       <c r="Y3" s="3"/>
       <c r="Z3" s="3"/>
     </row>
-    <row r="4" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F4" t="str">
         <f t="shared" si="0"/>
         <v>ST3</v>
@@ -3383,7 +3385,7 @@
         <v>13</v>
       </c>
     </row>
-    <row r="5" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F5" t="str">
         <f t="shared" si="0"/>
         <v>ST4</v>
@@ -3395,7 +3397,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="6" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F6" t="str">
         <f t="shared" si="0"/>
         <v>ST5</v>
@@ -3407,7 +3409,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F7" t="str">
         <f t="shared" si="0"/>
         <v>ST6</v>
@@ -3419,7 +3421,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="8" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F8" t="str">
         <f t="shared" si="0"/>
         <v>ST7</v>
@@ -3431,7 +3433,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F9" t="str">
         <f t="shared" si="0"/>
         <v>ST8</v>
@@ -3443,7 +3445,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="10" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>ST9</v>
@@ -3455,7 +3457,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="11" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F11" t="str">
         <f t="shared" si="0"/>
         <v>ST10</v>
@@ -3467,7 +3469,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="12" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F12" t="str">
         <f t="shared" si="0"/>
         <v>ST11</v>
@@ -3479,7 +3481,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="13" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F13" t="str">
         <f t="shared" si="0"/>
         <v>ST12</v>
@@ -3491,7 +3493,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="14" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F14" t="str">
         <f t="shared" si="0"/>
         <v>ST13</v>
@@ -3503,7 +3505,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="15" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F15" t="str">
         <f t="shared" si="0"/>
         <v>ST14</v>
@@ -3515,7 +3517,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="16" spans="2:26" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:26" x14ac:dyDescent="0.45">
       <c r="F16" t="str">
         <f t="shared" si="0"/>
         <v>ST15</v>
@@ -3527,7 +3529,7 @@
         <v>26</v>
       </c>
     </row>
-    <row r="17" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="17" spans="6:26" x14ac:dyDescent="0.45">
       <c r="F17" t="str">
         <f t="shared" si="0"/>
         <v>ST16</v>
@@ -3539,7 +3541,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="18" spans="6:26" x14ac:dyDescent="0.45">
       <c r="F18" t="str">
         <f t="shared" si="0"/>
         <v>ST17</v>
@@ -3551,7 +3553,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="19" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="19" spans="6:26" x14ac:dyDescent="0.45">
       <c r="F19" t="str">
         <f t="shared" si="0"/>
         <v>ST18</v>
@@ -3563,7 +3565,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="20" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="20" spans="6:26" x14ac:dyDescent="0.45">
       <c r="F20" t="str">
         <f t="shared" si="0"/>
         <v>ST19</v>
@@ -3575,7 +3577,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="21" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="21" spans="6:26" x14ac:dyDescent="0.45">
       <c r="F21" t="str">
         <f t="shared" si="0"/>
         <v>ST20</v>
@@ -3587,7 +3589,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="22" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="22" spans="6:26" x14ac:dyDescent="0.45">
       <c r="Y22" s="3">
         <v>19</v>
       </c>
@@ -3595,7 +3597,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="23" spans="6:26" x14ac:dyDescent="0.25">
+    <row r="23" spans="6:26" x14ac:dyDescent="0.45">
       <c r="Y23" s="3">
         <v>20</v>
       </c>
@@ -3603,7 +3605,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="195" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="195" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A195" t="s">
         <v>5</v>
       </c>
@@ -3617,7 +3619,7 @@
         <v>-1.4451000000000001</v>
       </c>
     </row>
-    <row r="196" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A196" t="s">
         <v>6</v>
       </c>
@@ -3652,19 +3654,19 @@
   <sheetPr codeName="Sheet6"/>
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B12" sqref="B12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D19" sqref="D19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.140625" style="4" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="10.7109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.1328125" style="4" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="10.73046875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="9.86328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>36</v>
       </c>
@@ -3678,13 +3680,13 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A2" t="str">
         <f>"ST"&amp;B2</f>
-        <v>ST1</v>
+        <v>ST2</v>
       </c>
       <c r="B2" s="4">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C2">
         <v>23</v>
@@ -3693,13 +3695,13 @@
         <v>45</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A3" t="str">
         <f t="shared" ref="A3:A5" si="0">"ST"&amp;B3</f>
-        <v>ST2</v>
+        <v>ST3</v>
       </c>
       <c r="B3" s="4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -3708,13 +3710,13 @@
         <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A4" t="str">
         <f t="shared" si="0"/>
-        <v>ST3</v>
+        <v>ST4</v>
       </c>
       <c r="B4" s="4">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="C4">
         <v>15</v>
@@ -3723,13 +3725,13 @@
         <v>60</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.45">
       <c r="A5" t="str">
         <f t="shared" si="0"/>
-        <v>ST4</v>
+        <v>ST6</v>
       </c>
       <c r="B5" s="4">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="C5">
         <v>100</v>
@@ -3749,16 +3751,16 @@
   <sheetPr codeName="Sheet7"/>
   <dimension ref="A1:AI15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="Q10" sqref="Q10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
-    <col min="1" max="1" width="16.28515625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="16.265625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A1" t="s">
         <v>41</v>
       </c>
@@ -3773,7 +3775,7 @@
       <c r="H1" s="10"/>
       <c r="I1" s="10"/>
     </row>
-    <row r="2" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:35" x14ac:dyDescent="0.45">
       <c r="B2" s="10" t="s">
         <v>42</v>
       </c>
@@ -3785,12 +3787,12 @@
       <c r="H2" s="10"/>
       <c r="I2" s="10"/>
     </row>
-    <row r="3" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A3" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A4">
         <v>1</v>
       </c>
@@ -3811,7 +3813,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="5" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:35" x14ac:dyDescent="0.45">
       <c r="D5">
         <v>1</v>
       </c>
@@ -3822,12 +3824,12 @@
         <v>48</v>
       </c>
     </row>
-    <row r="6" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:35" x14ac:dyDescent="0.45">
       <c r="J6" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A7" s="6" t="s">
         <v>47</v>
       </c>
@@ -3835,7 +3837,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="8" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A8" s="5" t="s">
         <v>40</v>
       </c>
@@ -3850,7 +3852,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="9" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A9" s="5" t="s">
         <v>3</v>
       </c>
@@ -3876,7 +3878,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A10" s="5" t="str">
         <f>"ST" &amp; N &amp; "_M_" &amp; M</f>
         <v>ST1_M_10</v>
@@ -3976,7 +3978,7 @@
         <v>0.80414884106932305</v>
       </c>
     </row>
-    <row r="11" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A11" s="8" t="s">
         <v>52</v>
       </c>
@@ -3984,12 +3986,12 @@
         <v>56</v>
       </c>
     </row>
-    <row r="12" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A12" s="6" t="s">
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A13" s="5" t="s">
         <v>13</v>
       </c>
@@ -4011,7 +4013,7 @@
       <c r="O13" s="5"/>
       <c r="P13" s="5"/>
     </row>
-    <row r="14" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A14" s="5" t="s">
         <v>3</v>
       </c>
@@ -4061,7 +4063,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:35" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:35" x14ac:dyDescent="0.45">
       <c r="A15" s="5" t="s">
         <v>39</v>
       </c>

</xml_diff>